<commit_message>
done gui for web
</commit_message>
<xml_diff>
--- a/excels/history.xlsx
+++ b/excels/history.xlsx
@@ -14,24 +14,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="3">
   <si>
-    <t>30-03-2018</t>
+    <t>08-05-2018</t>
   </si>
   <si>
     <t>12</t>
   </si>
   <si>
-    <t>23</t>
-  </si>
-  <si>
-    <t>21</t>
-  </si>
-  <si>
-    <t>41</t>
-  </si>
-  <si>
-    <t>23-02-2018</t>
+    <t>2</t>
   </si>
 </sst>
 </file>
@@ -367,7 +358,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A2:C5"/>
+  <dimension ref="A2:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -375,42 +366,22 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
       <c r="B2" t="s">
         <v>1</v>
       </c>
-      <c r="C2" t="s">
-        <v>2</v>
-      </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:2">
       <c r="B3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
-      <c r="A4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
-      <c r="B5" t="s">
         <v>2</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="1">
     <mergeCell ref="A2:A3"/>
-    <mergeCell ref="A4:A5"/>
   </mergeCells>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>

</xml_diff>